<commit_message>
primerBarcodeList: sql & ATGC composition breakdown
</commit_message>
<xml_diff>
--- a/data/indexed_primers/indexed_V4-V5_primers_db.xlsx
+++ b/data/indexed_primers/indexed_V4-V5_primers_db.xlsx
@@ -345,8 +345,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -366,15 +378,27 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -707,7 +731,7 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2161,7 +2185,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>21</v>
@@ -2271,7 +2295,7 @@
         <v>19</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>21</v>

</xml_diff>